<commit_message>
Monografia: bibliografia, siglas, cronograma, historias de usuario, protótipos foram finalizados; Criação das funções de atualizar e excluir funcionário, inicio do diagrama de classes
</commit_message>
<xml_diff>
--- a/#documentacao/Cronograma de tempo atividade.xlsx
+++ b/#documentacao/Cronograma de tempo atividade.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lolox\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Lanchonete-Mamaezona-TCC\#documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F831D66-688F-4B5C-BDA6-217DD9297756}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1707B2EF-9756-491A-BC37-CCC14B272EAD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7A85F87D-9C3C-41BE-9999-296F843D2D70}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{7A85F87D-9C3C-41BE-9999-296F843D2D70}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha2" sheetId="2" r:id="rId1"/>
@@ -703,8 +703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{625E9C0A-CD31-4971-8056-F22B978C6116}">
   <dimension ref="A1:W17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="Y17" sqref="Y17"/>
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>